<commit_message>
exploration, feature engineering, vt collections, encoding report
</commit_message>
<xml_diff>
--- a/false_positives/summary_df.xlsx
+++ b/false_positives/summary_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
         <v>1193385038.88</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -483,7 +483,7 @@
         <v>1193385038.88</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -501,11 +501,11 @@
         <v>1193385038.88</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>microgalon.com</t>
+          <t>solnicka.sk</t>
         </is>
       </c>
     </row>
@@ -519,65 +519,65 @@
         <v>1193385038.88</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>a.antlauncher.com</t>
+          <t>secureintellicentre.net.au</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1193385038.88</v>
+        <v>820368000</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>www.studiumarteterapie.cz</t>
+          <t>edoardocolombo.eu</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5077</v>
+        <v>820368000</v>
       </c>
       <c r="C7" t="n">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>www.zhcsm.cn</t>
+          <t>synapse.caterpillarcheesecake.xyz</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5077</v>
+        <v>820368000</v>
       </c>
       <c r="C8" t="n">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>smaxdn.com</t>
+          <t>www.studiumarteterapie.cz</t>
         </is>
       </c>
     </row>
@@ -591,11 +591,11 @@
         <v>5077</v>
       </c>
       <c r="C9" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>doogh.club</t>
+          <t>games4.qqgametimes.com</t>
         </is>
       </c>
     </row>
@@ -609,11 +609,11 @@
         <v>5077</v>
       </c>
       <c r="C10" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ffe390afd658c19dcbf707e0597b846d.de.whecloud.com</t>
+          <t>torrentsnows.com</t>
         </is>
       </c>
     </row>
@@ -627,11 +627,11 @@
         <v>5077</v>
       </c>
       <c r="C11" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>gomonetworks.com</t>
+          <t>auth.merrillcorp.com</t>
         </is>
       </c>
     </row>
@@ -645,11 +645,11 @@
         <v>5077</v>
       </c>
       <c r="C12" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>dopublicity.us</t>
+          <t>2makestorage.com</t>
         </is>
       </c>
     </row>
@@ -663,11 +663,11 @@
         <v>5077</v>
       </c>
       <c r="C13" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>api.helium.systems</t>
+          <t>airportus.info</t>
         </is>
       </c>
     </row>
@@ -681,11 +681,11 @@
         <v>5077</v>
       </c>
       <c r="C14" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ikoula.testdebit.info</t>
+          <t>backupaccount.com</t>
         </is>
       </c>
     </row>
@@ -699,11 +699,11 @@
         <v>5077</v>
       </c>
       <c r="C15" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>torrent-download.to</t>
+          <t>one.exness.link</t>
         </is>
       </c>
     </row>
@@ -717,11 +717,11 @@
         <v>5077</v>
       </c>
       <c r="C16" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>torrentsnows.com</t>
+          <t>api.wmkankan.com</t>
         </is>
       </c>
     </row>
@@ -735,11 +735,11 @@
         <v>5077</v>
       </c>
       <c r="C17" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>auth.merrillcorp.com</t>
+          <t>awrcaverybrstuktdybstr.com</t>
         </is>
       </c>
     </row>
@@ -753,11 +753,11 @@
         <v>5077</v>
       </c>
       <c r="C18" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>chishir.com</t>
+          <t>s.ktxtr.com</t>
         </is>
       </c>
     </row>
@@ -771,11 +771,11 @@
         <v>5077</v>
       </c>
       <c r="C19" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2makestorage.com</t>
+          <t>www.zhcsm.cn</t>
         </is>
       </c>
     </row>
@@ -789,11 +789,11 @@
         <v>5077</v>
       </c>
       <c r="C20" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>airportus.info</t>
+          <t>smaxdn.com</t>
         </is>
       </c>
     </row>
@@ -807,11 +807,11 @@
         <v>5077</v>
       </c>
       <c r="C21" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>r.blok.link</t>
+          <t>doogh.club</t>
         </is>
       </c>
     </row>
@@ -825,11 +825,11 @@
         <v>5077</v>
       </c>
       <c r="C22" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>connect.dewvpn.cc</t>
+          <t>torrent-download.to</t>
         </is>
       </c>
     </row>
@@ -843,11 +843,11 @@
         <v>5077</v>
       </c>
       <c r="C23" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>banno-online.jackhenry.bank</t>
+          <t>vid-play.com</t>
         </is>
       </c>
     </row>
@@ -861,11 +861,11 @@
         <v>5077</v>
       </c>
       <c r="C24" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>discordapp.page.link</t>
+          <t>chishir.com</t>
         </is>
       </c>
     </row>
@@ -879,11 +879,11 @@
         <v>5077</v>
       </c>
       <c r="C25" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>tools1000.com</t>
+          <t>audiotel.com.mx</t>
         </is>
       </c>
     </row>
@@ -897,11 +897,11 @@
         <v>5077</v>
       </c>
       <c r="C26" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>one.exness.link</t>
+          <t>r.blok.link</t>
         </is>
       </c>
     </row>
@@ -915,11 +915,11 @@
         <v>5077</v>
       </c>
       <c r="C27" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>www.centrumprenatalnidiagnostiky.cz</t>
+          <t>connect.dewvpn.cc</t>
         </is>
       </c>
     </row>
@@ -933,11 +933,11 @@
         <v>5077</v>
       </c>
       <c r="C28" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>vafrike.ru</t>
+          <t>discordapp.page.link</t>
         </is>
       </c>
     </row>
@@ -951,11 +951,11 @@
         <v>5077</v>
       </c>
       <c r="C29" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>site2text-2021.web.app</t>
+          <t>tools1000.com</t>
         </is>
       </c>
     </row>
@@ -969,11 +969,11 @@
         <v>5077</v>
       </c>
       <c r="C30" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>api.wmkankan.com</t>
+          <t>www.centrumprenatalnidiagnostiky.cz</t>
         </is>
       </c>
     </row>
@@ -987,11 +987,11 @@
         <v>5077</v>
       </c>
       <c r="C31" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>awrcaverybrstuktdybstr.com</t>
+          <t>vafrike.ru</t>
         </is>
       </c>
     </row>
@@ -1005,11 +1005,11 @@
         <v>5077</v>
       </c>
       <c r="C32" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>awecerybtuitbyatr.com</t>
+          <t>speedtest.lovelivesupport.com</t>
         </is>
       </c>
     </row>
@@ -1023,11 +1023,11 @@
         <v>5077</v>
       </c>
       <c r="C33" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>speed-app.com</t>
+          <t>ucmetrixa.info</t>
         </is>
       </c>
     </row>
@@ -1041,11 +1041,11 @@
         <v>5077</v>
       </c>
       <c r="C34" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>s.ktxtr.com</t>
+          <t>awecerybtuitbyatr.com</t>
         </is>
       </c>
     </row>
@@ -1059,11 +1059,11 @@
         <v>5077</v>
       </c>
       <c r="C35" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>static.doubleclick.ne</t>
+          <t>speed-app.com</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
         <v>5077</v>
       </c>
       <c r="C36" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
         <v>5077</v>
       </c>
       <c r="C37" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1113,7 +1113,7 @@
         <v>5077</v>
       </c>
       <c r="C38" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1131,11 +1131,11 @@
         <v>5077</v>
       </c>
       <c r="C39" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>gll-wifi-controller.co.uk</t>
+          <t>imagodd.com</t>
         </is>
       </c>
     </row>
@@ -1149,11 +1149,11 @@
         <v>5077</v>
       </c>
       <c r="C40" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>yggnode.cf</t>
+          <t>laocaifengxitong.cc</t>
         </is>
       </c>
     </row>
@@ -1167,11 +1167,11 @@
         <v>5077</v>
       </c>
       <c r="C41" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>bankinformation.1c.ru</t>
+          <t>browser.tvall.cn</t>
         </is>
       </c>
     </row>
@@ -1185,11 +1185,11 @@
         <v>5077</v>
       </c>
       <c r="C42" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>laocaifengxitong.cc</t>
+          <t>st-fakesysupgrade.fakevivo.com.cn</t>
         </is>
       </c>
     </row>
@@ -1203,11 +1203,11 @@
         <v>5077</v>
       </c>
       <c r="C43" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>rmfstream.pl</t>
+          <t>tag.contactatonce.co.uk</t>
         </is>
       </c>
     </row>
@@ -1221,11 +1221,11 @@
         <v>5077</v>
       </c>
       <c r="C44" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>browser.tvall.cn</t>
+          <t>ntp.voipyourphone.com</t>
         </is>
       </c>
     </row>
@@ -1239,11 +1239,11 @@
         <v>5077</v>
       </c>
       <c r="C45" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>takungpao.com.hk</t>
+          <t>tinyhoneybee.com</t>
         </is>
       </c>
     </row>
@@ -1257,11 +1257,11 @@
         <v>5077</v>
       </c>
       <c r="C46" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>st-fakesysupgrade.fakevivo.com.cn</t>
+          <t>update.xz0123.com</t>
         </is>
       </c>
     </row>
@@ -1275,11 +1275,11 @@
         <v>5077</v>
       </c>
       <c r="C47" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>tag.contactatonce.co.uk</t>
+          <t>aiacompanystore.com</t>
         </is>
       </c>
     </row>
@@ -1293,11 +1293,11 @@
         <v>5077</v>
       </c>
       <c r="C48" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>honda.usbsoftwareupdates.com</t>
+          <t>dinoyy.xyz</t>
         </is>
       </c>
     </row>
@@ -1311,11 +1311,11 @@
         <v>5077</v>
       </c>
       <c r="C49" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>tinyhoneybee.com</t>
+          <t>api.tinyhoneybee.com</t>
         </is>
       </c>
     </row>
@@ -1329,11 +1329,11 @@
         <v>5077</v>
       </c>
       <c r="C50" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>update.xz0123.com</t>
+          <t>www.cumonprintedpics.com</t>
         </is>
       </c>
     </row>
@@ -1347,11 +1347,11 @@
         <v>5077</v>
       </c>
       <c r="C51" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>ristekdikti.go.id</t>
+          <t>r9t1.com</t>
         </is>
       </c>
     </row>
@@ -1365,11 +1365,11 @@
         <v>5077</v>
       </c>
       <c r="C52" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>dinoyy.xyz</t>
+          <t>wincoolgifts.online</t>
         </is>
       </c>
     </row>
@@ -1383,11 +1383,11 @@
         <v>5077</v>
       </c>
       <c r="C53" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>forum.pcefans.cz</t>
+          <t>network-host.cf</t>
         </is>
       </c>
     </row>
@@ -1401,11 +1401,11 @@
         <v>5077</v>
       </c>
       <c r="C54" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>api.tinyhoneybee.com</t>
+          <t>eduid.ng</t>
         </is>
       </c>
     </row>
@@ -1419,11 +1419,11 @@
         <v>5077</v>
       </c>
       <c r="C55" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>wincoolgifts.online</t>
+          <t>cpestatus.seagateshare.com</t>
         </is>
       </c>
     </row>
@@ -1437,11 +1437,11 @@
         <v>5077</v>
       </c>
       <c r="C56" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>mygametoa.com</t>
+          <t>services.keepersecurity.eu</t>
         </is>
       </c>
     </row>
@@ -1455,11 +1455,11 @@
         <v>5077</v>
       </c>
       <c r="C57" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>cpestatus.seagateshare.com</t>
+          <t>www.shorturl.at</t>
         </is>
       </c>
     </row>
@@ -1473,11 +1473,11 @@
         <v>5077</v>
       </c>
       <c r="C58" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>www.shorturl.at</t>
+          <t>indigolbs.dinoyy.xyz</t>
         </is>
       </c>
     </row>
@@ -1491,11 +1491,11 @@
         <v>5077</v>
       </c>
       <c r="C59" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>indigolbs.dinoyy.xyz</t>
+          <t>escambiak12.edu</t>
         </is>
       </c>
     </row>
@@ -1509,11 +1509,11 @@
         <v>5077</v>
       </c>
       <c r="C60" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>escambiak12.edu</t>
+          <t>thor.prod.tvall.cn</t>
         </is>
       </c>
     </row>
@@ -1527,11 +1527,11 @@
         <v>5077</v>
       </c>
       <c r="C61" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>thor.prod.tvall.cn</t>
+          <t>60493198aa70ac43b4249ef4.endpoint.csper.io</t>
         </is>
       </c>
     </row>
@@ -1545,11 +1545,11 @@
         <v>5077</v>
       </c>
       <c r="C62" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>as-2314255.cdn.beampulse.com</t>
+          <t>wifihotspot.hu</t>
         </is>
       </c>
     </row>
@@ -1563,11 +1563,11 @@
         <v>5077</v>
       </c>
       <c r="C63" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>60493198aa70ac43b4249ef4.endpoint.csper.io</t>
+          <t>wikitextbooks.info</t>
         </is>
       </c>
     </row>
@@ -1581,11 +1581,11 @@
         <v>5077</v>
       </c>
       <c r="C64" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>wifihotspot.hu</t>
+          <t>smartstreet.shopinet.xyz</t>
         </is>
       </c>
     </row>
@@ -1599,11 +1599,11 @@
         <v>5077</v>
       </c>
       <c r="C65" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>smartstreet.shopinet.xyz</t>
+          <t>epiccareeverywhere.addenbrookes.nhs.uk</t>
         </is>
       </c>
     </row>
@@ -1617,11 +1617,11 @@
         <v>5077</v>
       </c>
       <c r="C66" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>imagodd.com</t>
+          <t>salesos.yqluck.com</t>
         </is>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
         <v>5077</v>
       </c>
       <c r="C67" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
         <v>1349</v>
       </c>
       <c r="C68" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -1671,7 +1671,7 @@
         <v>1349</v>
       </c>
       <c r="C69" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1689,11 +1689,11 @@
         <v>1349</v>
       </c>
       <c r="C70" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>onbase.space</t>
+          <t>ailanibah.com</t>
         </is>
       </c>
     </row>
@@ -1707,11 +1707,11 @@
         <v>1349</v>
       </c>
       <c r="C71" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>www.honestfoodtalks.com</t>
+          <t>onbase.space</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
         <v>1349</v>
       </c>
       <c r="C72" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -1736,90 +1736,90 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>rdap_ip_v4_count</t>
+          <t>tls_root_cert_validity_len</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>10</v>
+        <v>1349</v>
       </c>
       <c r="C73" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>baipiao-rss.com</t>
+          <t>call.easy2convert4.me</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>rdap_ip_v4_count</t>
+          <t>tls_root_cert_validity_len</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>10</v>
+        <v>1349</v>
       </c>
       <c r="C74" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>value-wolf.org</t>
+          <t>ytmp3.nu</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>rdap_ip_v4_count</t>
+          <t>dns_zone_len</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C75" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>tracker.sylphix.com</t>
+          <t>yggnode.cf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>rdap_ip_v4_count</t>
+          <t>dns_zone_len</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C76" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>p1prod.cardinalsupportconnect.com</t>
+          <t>farehitchlower.icu</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>rdap_ip_v4_count</t>
+          <t>dns_zone_len</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C77" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>iinmobi.com</t>
+          <t>up.surfsharking.com</t>
         </is>
       </c>
     </row>
@@ -1830,14 +1830,14 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C78" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>urchintelemetry.com</t>
+          <t>cba4a6e5d3c956548a337c52388473f1.com</t>
         </is>
       </c>
     </row>
@@ -1848,14 +1848,14 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C79" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>biblehu.com</t>
+          <t>baipiao-rss.com</t>
         </is>
       </c>
     </row>
@@ -1866,14 +1866,14 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C80" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>cdn.mypanel.link</t>
+          <t>value-wolf.org</t>
         </is>
       </c>
     </row>
@@ -1884,14 +1884,14 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C81" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>stun.zmzfile.com</t>
+          <t>iinmobi.com</t>
         </is>
       </c>
     </row>
@@ -1902,14 +1902,14 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C82" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>adblock-for-chrome.com</t>
+          <t>urchintelemetry.com</t>
         </is>
       </c>
     </row>
@@ -1920,14 +1920,14 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C83" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>services.labanquepostale.fr</t>
+          <t>biblehu.com</t>
         </is>
       </c>
     </row>
@@ -1938,14 +1938,14 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C84" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>matrix.matrixmsg.ml</t>
+          <t>cdn.mypanel.link</t>
         </is>
       </c>
     </row>
@@ -1956,14 +1956,14 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C85" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>www.vysocinaconvention.cz</t>
+          <t>cantliee.com</t>
         </is>
       </c>
     </row>
@@ -1974,14 +1974,14 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C86" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>accounts-account-service-prod.hydra.prod.wwrk.co</t>
+          <t>stun.zmzfile.com</t>
         </is>
       </c>
     </row>
@@ -1992,14 +1992,14 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C87" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>520camera.com</t>
+          <t>www.manpower.gov.om</t>
         </is>
       </c>
     </row>
@@ -2010,14 +2010,14 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C88" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>lt.logly.co.jp</t>
+          <t>accounts-account-service-prod.hydra.prod.wwrk.co</t>
         </is>
       </c>
     </row>
@@ -2028,14 +2028,14 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C89" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>smart.tinyhoneybee.com</t>
+          <t>lt.logly.co.jp</t>
         </is>
       </c>
     </row>
@@ -2046,14 +2046,14 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C90" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>api.html5media.info</t>
+          <t>smart.tinyhoneybee.com</t>
         </is>
       </c>
     </row>
@@ -2064,14 +2064,14 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C91" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>androidevlog.com</t>
+          <t>stat.speed-app.com</t>
         </is>
       </c>
     </row>
@@ -2082,86 +2082,86 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C92" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>addresseepaper.com</t>
+          <t>api.html5media.info</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>rdap_ip_v4_count</t>
+          <t>lex_malware_tetragram_matches</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C93" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>services.keepersecurity.eu</t>
+          <t>video.browser.tvall.cn</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>lex_malware_tetragram_matches</t>
+          <t>lex_avg_part_len</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>4</v>
+        <v>3.33</v>
       </c>
       <c r="C94" t="n">
         <v>1</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>video.browser.tvall.cn</t>
+          <t>advertisement.alibabacorp.sm.cn</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>lex_ipv4_in_domain</t>
+          <t>tls_joint_isoitu_policy_crt_count</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>up.surfsharking.com</t>
+          <t>ibaraki-84764.herokussl.com</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>lex_tld_abuse_score</t>
+          <t>tls_joint_isoitu_policy_crt_count</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.66</v>
+        <v>3</v>
       </c>
       <c r="C96" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>deliciouscheesesfromfrance.com</t>
+          <t>www.honestfoodtalks.com</t>
         </is>
       </c>
     </row>
@@ -2175,11 +2175,11 @@
         <v>0.66</v>
       </c>
       <c r="C97" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>nutrien-iksmedia-ccm.net</t>
+          <t>deliciouscheesesfromfrance.com</t>
         </is>
       </c>
     </row>
@@ -2193,11 +2193,11 @@
         <v>0.66</v>
       </c>
       <c r="C98" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>www.zf.ro</t>
+          <t>gll-wifi-controller.co.uk</t>
         </is>
       </c>
     </row>
@@ -2211,11 +2211,11 @@
         <v>0.66</v>
       </c>
       <c r="C99" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>sunofgodd.com</t>
+          <t>nutrien-iksmedia-ccm.net</t>
         </is>
       </c>
     </row>
@@ -2229,11 +2229,11 @@
         <v>0.66</v>
       </c>
       <c r="C100" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>api.video.browser.tvall.cn</t>
+          <t>www.zf.ro</t>
         </is>
       </c>
     </row>
@@ -2247,11 +2247,11 @@
         <v>0.66</v>
       </c>
       <c r="C101" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>laryngectomy.cultivateward.eu</t>
+          <t>matrix.matrixmsg.ml</t>
         </is>
       </c>
     </row>
@@ -2265,11 +2265,11 @@
         <v>0.66</v>
       </c>
       <c r="C102" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>cpa-optimizer.online</t>
+          <t>deeponlines.com</t>
         </is>
       </c>
     </row>
@@ -2283,11 +2283,11 @@
         <v>0.66</v>
       </c>
       <c r="C103" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>www.cumonprintedpics.com</t>
+          <t>api.video.browser.tvall.cn</t>
         </is>
       </c>
     </row>
@@ -2301,11 +2301,11 @@
         <v>0.66</v>
       </c>
       <c r="C104" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>www.qqgametimes.com</t>
+          <t>laryngectomy.cultivateward.eu</t>
         </is>
       </c>
     </row>
@@ -2319,11 +2319,11 @@
         <v>0.66</v>
       </c>
       <c r="C105" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>checkmytrip.app.link</t>
+          <t>api.zcoup.com</t>
         </is>
       </c>
     </row>
@@ -2337,11 +2337,11 @@
         <v>0.66</v>
       </c>
       <c r="C106" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>www.simplywhisked.com</t>
+          <t>androidevlog.com</t>
         </is>
       </c>
     </row>
@@ -2355,11 +2355,11 @@
         <v>0.66</v>
       </c>
       <c r="C107" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>gpvjyx.ssptp4.com</t>
+          <t>www.qqgametimes.com</t>
         </is>
       </c>
     </row>
@@ -2373,11 +2373,11 @@
         <v>0.66</v>
       </c>
       <c r="C108" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>blessifyinfotech.com</t>
+          <t>gpvjyx.ssptp4.com</t>
         </is>
       </c>
     </row>
@@ -2391,11 +2391,11 @@
         <v>0.66</v>
       </c>
       <c r="C109" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>edoardocolombo.eu</t>
+          <t>addresseepaper.com</t>
         </is>
       </c>
     </row>
@@ -2409,11 +2409,11 @@
         <v>0.66</v>
       </c>
       <c r="C110" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>ulfbrueggemann.no-ip.org</t>
+          <t>avt-usa.net</t>
         </is>
       </c>
     </row>
@@ -2427,11 +2427,11 @@
         <v>0.66</v>
       </c>
       <c r="C111" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>legitville.com</t>
+          <t>blessifyinfotech.com</t>
         </is>
       </c>
     </row>
@@ -2445,11 +2445,11 @@
         <v>0.66</v>
       </c>
       <c r="C112" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>raisingteenstoday.com</t>
+          <t>ulfbrueggemann.no-ip.org</t>
         </is>
       </c>
     </row>
@@ -2463,11 +2463,11 @@
         <v>0.66</v>
       </c>
       <c r="C113" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>advertisement.alibabacorp.sm.cn</t>
+          <t>toubiz.de</t>
         </is>
       </c>
     </row>
@@ -2481,155 +2481,155 @@
         <v>0.66</v>
       </c>
       <c r="C114" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>cygnetinfotechmanagedservices.com</t>
+          <t>legitville.com</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>lex_tld_abuse_score</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.53</v>
+        <v>0.66</v>
       </c>
       <c r="C115" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>farehitchlower.icu</t>
+          <t>www.blogpeople.net</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>lex_tld_abuse_score</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.53</v>
+        <v>0.66</v>
       </c>
       <c r="C116" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>rock.fotapro.com</t>
+          <t>raisingteenstoday.com</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>lex_tld_abuse_score</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.53</v>
+        <v>0.66</v>
       </c>
       <c r="C117" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>mk-beta.ru</t>
+          <t>hkoptimize.com</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>lex_tld_abuse_score</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.53</v>
+        <v>0.66</v>
       </c>
       <c r="C118" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>hkoptimize.com</t>
+          <t>cygnetinfotechmanagedservices.com</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>rdap_registrar_name_hash</t>
+          <t>dns_ttl_low</t>
         </is>
       </c>
       <c r="B119" t="n">
         <v>0</v>
       </c>
       <c r="C119" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>deeponlines.com</t>
+          <t>www.eye-able-cdn.com</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>rdap_registrar_name_hash</t>
+          <t>dns_ttl_low</t>
         </is>
       </c>
       <c r="B120" t="n">
         <v>0</v>
       </c>
       <c r="C120" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>solnicka.sk</t>
+          <t>mail.wavela.bid</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>rdap_registrar_name_hash</t>
+          <t>dns_ttl_low</t>
         </is>
       </c>
       <c r="B121" t="n">
         <v>0</v>
       </c>
       <c r="C121" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>wmkankan.com</t>
+          <t>tracker.sylphix.com</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>rdap_registrar_name_hash</t>
+          <t>dns_ttl_low</t>
         </is>
       </c>
       <c r="B122" t="n">
         <v>0</v>
       </c>
       <c r="C122" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>adtaginformer.com</t>
+          <t>www.adtaginformer.com</t>
         </is>
       </c>
     </row>
@@ -2643,11 +2643,11 @@
         <v>0</v>
       </c>
       <c r="C123" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>www.adtaginformer.com</t>
+          <t>logoff.fr</t>
         </is>
       </c>
     </row>
@@ -2661,11 +2661,11 @@
         <v>0</v>
       </c>
       <c r="C124" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>johnrosen1.com</t>
+          <t>ginrummyandgames.com</t>
         </is>
       </c>
     </row>
@@ -2679,11 +2679,11 @@
         <v>0</v>
       </c>
       <c r="C125" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>nasscom-live.com</t>
+          <t>g3telecompi.com.br</t>
         </is>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="C126" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -2708,32 +2708,54 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr"/>
+          <t>dns_ttl_avg</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>0</v>
+      </c>
       <c r="C127" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>ibaraki-84764.herokussl.com</t>
+          <t>a.antlauncher.com</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr"/>
+          <t>rdap_registrar_name_hash</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>0</v>
+      </c>
       <c r="C128" t="n">
         <v>2</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>api.zcoup.com</t>
+          <t>wmkankan.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>rdap_registrar_name_hash</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>0</v>
+      </c>
+      <c r="C129" t="n">
+        <v>2</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>adtaginformer.com</t>
         </is>
       </c>
     </row>

</xml_diff>